<commit_message>
Update Kurs ohne Where!!!!
</commit_message>
<xml_diff>
--- a/Taetigkeitsprotokolle/Taetigkeitsprotokoll_Reiter.xlsx
+++ b/Taetigkeitsprotokolle/Taetigkeitsprotokoll_Reiter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Schule\5AHWII\SWP\Projekt\Ferienspass\Taetigkeitsprotokolle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AB485B-F83F-455A-9DCD-92711361691C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF946CE-6610-4C62-B0CE-4F2E4B772164}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="882" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>Datum</t>
   </si>
@@ -96,10 +96,34 @@
     <t>26.11.2019</t>
   </si>
   <si>
-    <t>Programming</t>
-  </si>
-  <si>
     <t>03.12.2019</t>
+  </si>
+  <si>
+    <t>stylesheet, Registrierung, Password-Class, Logout, Weiterleitung Registrierung</t>
+  </si>
+  <si>
+    <t>Masterunterscheidung User/Admin, Passwort-Überprüfung, E-Mail-Klasse, AGBs und DsGV, Logout-Button, Weiterleitung Passwort vergessen</t>
+  </si>
+  <si>
+    <t>10.12.2019</t>
+  </si>
+  <si>
+    <t>Kurse anzeigen+anlegen</t>
+  </si>
+  <si>
+    <t>Mi</t>
+  </si>
+  <si>
+    <t>11.12.2019</t>
+  </si>
+  <si>
+    <t>Kurs anlegen</t>
+  </si>
+  <si>
+    <t>17.12.2019</t>
+  </si>
+  <si>
+    <t>7.1.2020</t>
   </si>
 </sst>
 </file>
@@ -297,6 +321,18 @@
     <xf numFmtId="166" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -320,18 +356,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -732,7 +756,7 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -745,12 +769,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="8"/>
@@ -787,35 +811,35 @@
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="31" t="s">
+      <c r="B5" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="35" t="s">
+      <c r="D5" s="35"/>
+      <c r="E5" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="39" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:13" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="8"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
@@ -867,12 +891,12 @@
         <v>8.333333333333337E-2</v>
       </c>
       <c r="G8" s="11"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
     </row>
     <row r="9" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
@@ -897,7 +921,7 @@
       <c r="G9" s="11"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>15</v>
       </c>
@@ -911,7 +935,7 @@
         <v>0.54861111111111105</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F10" s="26">
         <f t="shared" si="0"/>
@@ -925,7 +949,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="25">
         <v>0.32291666666666669</v>
@@ -934,7 +958,7 @@
         <v>0.54861111111111105</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F11" s="26">
         <f t="shared" si="0"/>
@@ -943,50 +967,90 @@
       <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="27"/>
+      <c r="A12" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="25">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="D12" s="25">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>25</v>
+      </c>
       <c r="F12" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.22569444444444436</v>
       </c>
       <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="27"/>
+      <c r="A13" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="25">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D13" s="25">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>28</v>
+      </c>
       <c r="F13" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9444444444444531E-2</v>
       </c>
       <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="27"/>
+      <c r="A14" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="25">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="D14" s="25">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>28</v>
+      </c>
       <c r="F14" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.22569444444444436</v>
       </c>
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="27"/>
+      <c r="A15" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="25">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="D15" s="25">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>28</v>
+      </c>
       <c r="F15" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.22569444444444436</v>
       </c>
       <c r="G15" s="11"/>
     </row>
@@ -1257,109 +1321,109 @@
       <c r="G37" s="11"/>
     </row>
     <row r="38" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="22">
         <f>SUM(F7:F37)</f>
-        <v>0.82986111111111094</v>
+        <v>1.5763888888888888</v>
       </c>
       <c r="G38" s="8"/>
     </row>
     <row r="39" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="38"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
       <c r="G39" s="8"/>
     </row>
     <row r="40" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
       <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="39"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
+      <c r="A41" s="31"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
       <c r="G41" s="8"/>
     </row>
     <row r="42" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="40"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
+      <c r="A42" s="32"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
       <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="37"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
+      <c r="A43" s="29"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
       <c r="G43" s="8"/>
     </row>
     <row r="44" spans="1:7" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="37"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
       <c r="G44" s="8"/>
     </row>
     <row r="45" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="37"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
+      <c r="A45" s="29"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
       <c r="G45" s="8"/>
     </row>
     <row r="46" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="37"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
+      <c r="A46" s="29"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
       <c r="G46" s="8"/>
     </row>
     <row r="47" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="37"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
+      <c r="A47" s="29"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
       <c r="G47" s="8"/>
     </row>
     <row r="48" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="37"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
+      <c r="A48" s="29"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
       <c r="G48" s="8"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1382,6 +1446,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="A46:F46"/>
     <mergeCell ref="A47:F47"/>
     <mergeCell ref="A48:F48"/>
@@ -1391,15 +1464,6 @@
     <mergeCell ref="A43:F43"/>
     <mergeCell ref="A44:F44"/>
     <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="H8:M8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Send Mail to Participants of Course
</commit_message>
<xml_diff>
--- a/Taetigkeitsprotokolle/Taetigkeitsprotokoll_Reiter.xlsx
+++ b/Taetigkeitsprotokolle/Taetigkeitsprotokoll_Reiter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Schule\5AHWII\SWP\Projekt\Ferienspass\Taetigkeitsprotokolle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF946CE-6610-4C62-B0CE-4F2E4B772164}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACAE8C6-BF18-416B-8E13-CDDCDC972C7F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="882" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Datum</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>7.1.2020</t>
+  </si>
+  <si>
+    <t>Kurs anlegen, Kurs bearbeiten, Mail an Teilnehmer im Kurs versenden, Validate</t>
   </si>
 </sst>
 </file>
@@ -321,6 +324,30 @@
     <xf numFmtId="166" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -332,30 +359,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -756,7 +759,7 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -769,12 +772,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="8"/>
@@ -811,35 +814,35 @@
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="35" t="s">
+      <c r="B5" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="39" t="s">
+      <c r="D5" s="31"/>
+      <c r="E5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="35" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:13" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="8"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
@@ -891,12 +894,12 @@
         <v>8.333333333333337E-2</v>
       </c>
       <c r="G8" s="11"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
     </row>
     <row r="9" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
@@ -1032,7 +1035,7 @@
       </c>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>15</v>
       </c>
@@ -1046,7 +1049,7 @@
         <v>0.54861111111111105</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F15" s="26">
         <f t="shared" si="0"/>
@@ -1321,13 +1324,13 @@
       <c r="G37" s="11"/>
     </row>
     <row r="38" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="33" t="s">
+      <c r="A38" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="33"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="22">
         <f>SUM(F7:F37)</f>
         <v>1.5763888888888888</v>
@@ -1335,95 +1338,95 @@
       <c r="G38" s="8"/>
     </row>
     <row r="39" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
+      <c r="A39" s="38"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
       <c r="G39" s="8"/>
     </row>
     <row r="40" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="34" t="s">
+      <c r="A40" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
       <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
       <c r="G41" s="8"/>
     </row>
     <row r="42" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="32"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="32"/>
+      <c r="A42" s="40"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
       <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
+      <c r="A43" s="37"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
       <c r="G43" s="8"/>
     </row>
     <row r="44" spans="1:7" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
+      <c r="A44" s="37"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
       <c r="G44" s="8"/>
     </row>
     <row r="45" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
+      <c r="A45" s="37"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
       <c r="G45" s="8"/>
     </row>
     <row r="46" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
       <c r="G46" s="8"/>
     </row>
     <row r="47" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="29"/>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
+      <c r="A47" s="37"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
       <c r="G47" s="8"/>
     </row>
     <row r="48" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="29"/>
-      <c r="B48" s="29"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
+      <c r="A48" s="37"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
       <c r="G48" s="8"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1446,6 +1449,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A45:F45"/>
     <mergeCell ref="A38:E38"/>
     <mergeCell ref="A40:F40"/>
     <mergeCell ref="C5:D5"/>
@@ -1455,15 +1467,6 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A45:F45"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>